<commit_message>
Concat operator mode added to Delphi version, Excel charts updated
</commit_message>
<xml_diff>
--- a/Results/StringBuilder.xlsx
+++ b/Results/StringBuilder.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>Repeat</t>
   </si>
@@ -25,16 +25,19 @@
     <t>Subtotal</t>
   </si>
   <si>
-    <t>.NET 3.5</t>
+    <t>K             N</t>
   </si>
   <si>
-    <t>.NET 4.5</t>
+    <t>Delphi XE3 (+)</t>
   </si>
   <si>
-    <t>Delphi XE3</t>
+    <t>Delphi XE3 (TStringBuilder)</t>
   </si>
   <si>
-    <t>K             N</t>
+    <t>.NET 4.5 (StringBuilder)</t>
+  </si>
+  <si>
+    <t>.NET 3.5 (StringBuilder)</t>
   </si>
 </sst>
 </file>
@@ -372,11 +375,13 @@
     <xf numFmtId="3" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -386,13 +391,11 @@
     <xf numFmtId="3" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -695,7 +698,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O42"/>
+  <dimension ref="B2:AB28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -704,25 +707,40 @@
     <col min="1" max="1" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
+    <row r="2" spans="2:28" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="P2" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
     </row>
-    <row r="3" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -731,25 +749,48 @@
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="25"/>
-      <c r="F4" s="26">
+      <c r="F4" s="19">
         <v>100</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="26">
+      <c r="G4" s="20"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="19">
         <v>10000</v>
       </c>
-      <c r="J4" s="27"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="26">
+      <c r="J4" s="20"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="19">
         <v>1000000</v>
       </c>
-      <c r="M4" s="27"/>
-      <c r="N4" s="29"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="22"/>
+      <c r="P4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="23">
+        <v>1</v>
+      </c>
+      <c r="R4" s="24"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="19">
+        <v>100</v>
+      </c>
+      <c r="U4" s="20"/>
+      <c r="V4" s="21"/>
+      <c r="W4" s="19">
+        <v>10000</v>
+      </c>
+      <c r="X4" s="20"/>
+      <c r="Y4" s="21"/>
+      <c r="Z4" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="AA4" s="20"/>
+      <c r="AB4" s="22"/>
     </row>
-    <row r="5" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="16" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C5" s="12">
         <v>1</v>
@@ -787,8 +828,47 @@
       <c r="N5" s="14">
         <v>4</v>
       </c>
+      <c r="P5" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="12">
+        <v>1</v>
+      </c>
+      <c r="R5" s="12">
+        <v>2</v>
+      </c>
+      <c r="S5" s="12">
+        <v>4</v>
+      </c>
+      <c r="T5" s="13">
+        <v>1</v>
+      </c>
+      <c r="U5" s="12">
+        <v>2</v>
+      </c>
+      <c r="V5" s="12">
+        <v>4</v>
+      </c>
+      <c r="W5" s="13">
+        <v>1</v>
+      </c>
+      <c r="X5" s="12">
+        <v>2</v>
+      </c>
+      <c r="Y5" s="12">
+        <v>4</v>
+      </c>
+      <c r="Z5" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="12">
+        <v>2</v>
+      </c>
+      <c r="AB5" s="14">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B6" s="15">
         <v>1</v>
       </c>
@@ -828,8 +908,47 @@
       <c r="N6" s="9">
         <v>8841</v>
       </c>
+      <c r="P6" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>16068</v>
+      </c>
+      <c r="R6" s="7">
+        <v>20795</v>
+      </c>
+      <c r="S6" s="7">
+        <v>33681</v>
+      </c>
+      <c r="T6" s="8">
+        <v>5273</v>
+      </c>
+      <c r="U6" s="7">
+        <v>9547</v>
+      </c>
+      <c r="V6" s="7">
+        <v>16941</v>
+      </c>
+      <c r="W6" s="8">
+        <v>4945</v>
+      </c>
+      <c r="X6" s="7">
+        <v>9048</v>
+      </c>
+      <c r="Y6" s="7">
+        <v>17456</v>
+      </c>
+      <c r="Z6" s="8">
+        <v>5164</v>
+      </c>
+      <c r="AA6" s="7">
+        <v>10031</v>
+      </c>
+      <c r="AB6" s="9">
+        <v>24212</v>
+      </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B7" s="15">
         <v>2</v>
       </c>
@@ -869,8 +988,47 @@
       <c r="N7" s="9">
         <v>15600</v>
       </c>
+      <c r="P7" s="15">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>16006</v>
+      </c>
+      <c r="R7" s="7">
+        <v>20670</v>
+      </c>
+      <c r="S7" s="7">
+        <v>42167</v>
+      </c>
+      <c r="T7" s="8">
+        <v>5398</v>
+      </c>
+      <c r="U7" s="7">
+        <v>9797</v>
+      </c>
+      <c r="V7" s="7">
+        <v>17894</v>
+      </c>
+      <c r="W7" s="8">
+        <v>5008</v>
+      </c>
+      <c r="X7" s="7">
+        <v>9126</v>
+      </c>
+      <c r="Y7" s="7">
+        <v>22168</v>
+      </c>
+      <c r="Z7" s="8">
+        <v>5476</v>
+      </c>
+      <c r="AA7" s="7">
+        <v>11123</v>
+      </c>
+      <c r="AB7" s="9">
+        <v>33197</v>
+      </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B8" s="15">
         <v>5</v>
       </c>
@@ -910,8 +1068,47 @@
       <c r="N8" s="9">
         <v>36589</v>
       </c>
+      <c r="P8" s="15">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>16099</v>
+      </c>
+      <c r="R8" s="7">
+        <v>19141</v>
+      </c>
+      <c r="S8" s="7">
+        <v>34148</v>
+      </c>
+      <c r="T8" s="8">
+        <v>5647</v>
+      </c>
+      <c r="U8" s="7">
+        <v>9454</v>
+      </c>
+      <c r="V8" s="7">
+        <v>20077</v>
+      </c>
+      <c r="W8" s="8">
+        <v>5195</v>
+      </c>
+      <c r="X8" s="7">
+        <v>9719</v>
+      </c>
+      <c r="Y8" s="7">
+        <v>33431</v>
+      </c>
+      <c r="Z8" s="8">
+        <v>7083</v>
+      </c>
+      <c r="AA8" s="7">
+        <v>13213</v>
+      </c>
+      <c r="AB8" s="9">
+        <v>49422</v>
+      </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B9" s="15">
         <v>10</v>
       </c>
@@ -951,8 +1148,47 @@
       <c r="N9" s="9">
         <v>71454</v>
       </c>
+      <c r="P9" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q9" s="7">
+        <v>16099</v>
+      </c>
+      <c r="R9" s="7">
+        <v>26442</v>
+      </c>
+      <c r="S9" s="7">
+        <v>40280</v>
+      </c>
+      <c r="T9" s="8">
+        <v>5975</v>
+      </c>
+      <c r="U9" s="7">
+        <v>10265</v>
+      </c>
+      <c r="V9" s="7">
+        <v>24492</v>
+      </c>
+      <c r="W9" s="8">
+        <v>5522</v>
+      </c>
+      <c r="X9" s="7">
+        <v>14134</v>
+      </c>
+      <c r="Y9" s="7">
+        <v>61183</v>
+      </c>
+      <c r="Z9" s="8">
+        <v>9360</v>
+      </c>
+      <c r="AA9" s="7">
+        <v>18657</v>
+      </c>
+      <c r="AB9" s="9">
+        <v>84241</v>
+      </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B10" s="15">
         <v>20</v>
       </c>
@@ -984,8 +1220,39 @@
         <v>23292</v>
       </c>
       <c r="N10" s="11"/>
+      <c r="P10" s="15">
+        <v>20</v>
+      </c>
+      <c r="Q10" s="7">
+        <v>23306</v>
+      </c>
+      <c r="R10" s="7">
+        <v>35724</v>
+      </c>
+      <c r="S10" s="10"/>
+      <c r="T10" s="8">
+        <v>6583</v>
+      </c>
+      <c r="U10" s="7">
+        <v>11731</v>
+      </c>
+      <c r="V10" s="10"/>
+      <c r="W10" s="8">
+        <v>7051</v>
+      </c>
+      <c r="X10" s="7">
+        <v>25038</v>
+      </c>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="8">
+        <v>14259</v>
+      </c>
+      <c r="AA10" s="7">
+        <v>29266</v>
+      </c>
+      <c r="AB10" s="11"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B11" s="15">
         <v>50</v>
       </c>
@@ -1017,8 +1284,39 @@
         <v>57952</v>
       </c>
       <c r="N11" s="11"/>
+      <c r="P11" s="15">
+        <v>50</v>
+      </c>
+      <c r="Q11" s="7">
+        <v>24898</v>
+      </c>
+      <c r="R11" s="7">
+        <v>37799</v>
+      </c>
+      <c r="S11" s="10"/>
+      <c r="T11" s="8">
+        <v>7878</v>
+      </c>
+      <c r="U11" s="7">
+        <v>16193</v>
+      </c>
+      <c r="V11" s="10"/>
+      <c r="W11" s="8">
+        <v>18003</v>
+      </c>
+      <c r="X11" s="7">
+        <v>47721</v>
+      </c>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="8">
+        <v>21871</v>
+      </c>
+      <c r="AA11" s="7">
+        <v>69967</v>
+      </c>
+      <c r="AB11" s="11"/>
     </row>
-    <row r="12" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="15">
         <v>100</v>
       </c>
@@ -1042,8 +1340,31 @@
       </c>
       <c r="M12" s="10"/>
       <c r="N12" s="11"/>
+      <c r="P12" s="15">
+        <v>100</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>26739</v>
+      </c>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="8">
+        <v>10156</v>
+      </c>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="8">
+        <v>38532</v>
+      </c>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="8">
+        <v>38969</v>
+      </c>
+      <c r="AA12" s="10"/>
+      <c r="AB12" s="11"/>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>2</v>
       </c>
@@ -1095,55 +1416,148 @@
         <f t="shared" si="0"/>
         <v>1.5333796296296295E-3</v>
       </c>
+      <c r="P13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="4">
+        <f t="shared" ref="Q13:AB13" si="1">SUM(Q6:Q12)/86400000</f>
+        <v>1.6112847222222223E-3</v>
+      </c>
+      <c r="R13" s="4">
+        <f t="shared" si="1"/>
+        <v>1.8584606481481481E-3</v>
+      </c>
+      <c r="S13" s="5">
+        <f t="shared" si="1"/>
+        <v>1.7393055555555556E-3</v>
+      </c>
+      <c r="T13" s="4">
+        <f t="shared" si="1"/>
+        <v>5.4293981481481478E-4</v>
+      </c>
+      <c r="U13" s="4">
+        <f t="shared" si="1"/>
+        <v>7.7531249999999996E-4</v>
+      </c>
+      <c r="V13" s="5">
+        <f t="shared" si="1"/>
+        <v>9.1902777777777772E-4</v>
+      </c>
+      <c r="W13" s="4">
+        <f t="shared" si="1"/>
+        <v>9.7518518518518516E-4</v>
+      </c>
+      <c r="X13" s="4">
+        <f t="shared" si="1"/>
+        <v>1.3285416666666667E-3</v>
+      </c>
+      <c r="Y13" s="5">
+        <f t="shared" si="1"/>
+        <v>1.5536805555555555E-3</v>
+      </c>
+      <c r="Z13" s="4">
+        <f t="shared" si="1"/>
+        <v>1.182662037037037E-3</v>
+      </c>
+      <c r="AA13" s="4">
+        <f t="shared" si="1"/>
+        <v>1.7622337962962962E-3</v>
+      </c>
+      <c r="AB13" s="6">
+        <f t="shared" si="1"/>
+        <v>2.2114814814814814E-3</v>
+      </c>
     </row>
-    <row r="14" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="26">
         <f>SUM(C13:E13)</f>
         <v>2.2150115740740741E-3</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="21">
+      <c r="D14" s="27"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="29">
         <f>SUM(F13:H13)</f>
         <v>9.4211805555555542E-4</v>
       </c>
-      <c r="G14" s="19"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="21">
+      <c r="G14" s="27"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="29">
         <f>SUM(I13:K13)</f>
         <v>1.7703935185185186E-3</v>
       </c>
-      <c r="J14" s="19"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="21">
+      <c r="J14" s="27"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="29">
         <f>SUM(L13:N13)</f>
         <v>3.5719675925925927E-3</v>
       </c>
-      <c r="M14" s="19"/>
-      <c r="N14" s="22"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="30"/>
+      <c r="P14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="26">
+        <f>SUM(Q13:S13)</f>
+        <v>5.209050925925926E-3</v>
+      </c>
+      <c r="R14" s="27"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="29">
+        <f>SUM(T13:V13)</f>
+        <v>2.2372800925925924E-3</v>
+      </c>
+      <c r="U14" s="27"/>
+      <c r="V14" s="28"/>
+      <c r="W14" s="29">
+        <f>SUM(W13:Y13)</f>
+        <v>3.8574074074074075E-3</v>
+      </c>
+      <c r="X14" s="27"/>
+      <c r="Y14" s="28"/>
+      <c r="Z14" s="29">
+        <f>SUM(Z13:AB13)</f>
+        <v>5.156377314814815E-3</v>
+      </c>
+      <c r="AA14" s="27"/>
+      <c r="AB14" s="30"/>
     </row>
-    <row r="16" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30"/>
+    <row r="16" spans="2:28" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="P16" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="18"/>
+      <c r="S16" s="18"/>
+      <c r="T16" s="18"/>
+      <c r="U16" s="18"/>
+      <c r="V16" s="18"/>
+      <c r="W16" s="18"/>
+      <c r="X16" s="18"/>
+      <c r="Y16" s="18"/>
+      <c r="Z16" s="18"/>
+      <c r="AA16" s="18"/>
+      <c r="AB16" s="18"/>
     </row>
-    <row r="17" spans="2:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>0</v>
       </c>
@@ -1152,25 +1566,48 @@
       </c>
       <c r="D18" s="24"/>
       <c r="E18" s="25"/>
-      <c r="F18" s="26">
+      <c r="F18" s="19">
         <v>100</v>
       </c>
-      <c r="G18" s="27"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="26">
+      <c r="G18" s="20"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="19">
         <v>10000</v>
       </c>
-      <c r="J18" s="27"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="26">
+      <c r="J18" s="20"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="19">
         <v>1000000</v>
       </c>
-      <c r="M18" s="27"/>
-      <c r="N18" s="29"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="22"/>
+      <c r="P18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="23">
+        <v>1</v>
+      </c>
+      <c r="R18" s="24"/>
+      <c r="S18" s="25"/>
+      <c r="T18" s="19">
+        <v>100</v>
+      </c>
+      <c r="U18" s="20"/>
+      <c r="V18" s="21"/>
+      <c r="W18" s="19">
+        <v>10000</v>
+      </c>
+      <c r="X18" s="20"/>
+      <c r="Y18" s="21"/>
+      <c r="Z18" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="AA18" s="20"/>
+      <c r="AB18" s="22"/>
     </row>
-    <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="16" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C19" s="12">
         <v>1</v>
@@ -1208,781 +1645,730 @@
       <c r="N19" s="14">
         <v>4</v>
       </c>
+      <c r="P19" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q19" s="12">
+        <v>1</v>
+      </c>
+      <c r="R19" s="12">
+        <v>2</v>
+      </c>
+      <c r="S19" s="12">
+        <v>4</v>
+      </c>
+      <c r="T19" s="13">
+        <v>1</v>
+      </c>
+      <c r="U19" s="12">
+        <v>2</v>
+      </c>
+      <c r="V19" s="12">
+        <v>4</v>
+      </c>
+      <c r="W19" s="13">
+        <v>1</v>
+      </c>
+      <c r="X19" s="12">
+        <v>2</v>
+      </c>
+      <c r="Y19" s="12">
+        <v>4</v>
+      </c>
+      <c r="Z19" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="12">
+        <v>2</v>
+      </c>
+      <c r="AB19" s="14">
+        <v>4</v>
+      </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B20" s="15">
         <v>1</v>
       </c>
       <c r="C20" s="7">
-        <v>16068</v>
+        <v>6555</v>
       </c>
       <c r="D20" s="7">
-        <v>20795</v>
+        <v>8065</v>
       </c>
       <c r="E20" s="7">
-        <v>33681</v>
+        <v>13054</v>
       </c>
       <c r="F20" s="8">
-        <v>5273</v>
+        <v>2385</v>
       </c>
       <c r="G20" s="7">
-        <v>9547</v>
+        <v>3872</v>
       </c>
       <c r="H20" s="7">
-        <v>16941</v>
+        <v>7894</v>
       </c>
       <c r="I20" s="8">
-        <v>4945</v>
+        <v>2354</v>
       </c>
       <c r="J20" s="7">
-        <v>9048</v>
+        <v>3649</v>
       </c>
       <c r="K20" s="7">
-        <v>17456</v>
+        <v>9393</v>
       </c>
       <c r="L20" s="8">
-        <v>5164</v>
+        <v>2397</v>
       </c>
       <c r="M20" s="7">
-        <v>10031</v>
+        <v>4029</v>
       </c>
       <c r="N20" s="9">
-        <v>24212</v>
+        <v>11527</v>
+      </c>
+      <c r="P20" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="7">
+        <v>6240</v>
+      </c>
+      <c r="R20" s="7">
+        <v>10670</v>
+      </c>
+      <c r="S20" s="7">
+        <v>18049</v>
+      </c>
+      <c r="T20" s="8">
+        <v>4695</v>
+      </c>
+      <c r="U20" s="7">
+        <v>8876</v>
+      </c>
+      <c r="V20" s="7">
+        <v>15756</v>
+      </c>
+      <c r="W20" s="8">
+        <v>4712</v>
+      </c>
+      <c r="X20" s="7">
+        <v>8830</v>
+      </c>
+      <c r="Y20" s="7">
+        <v>16536</v>
+      </c>
+      <c r="Z20" s="8">
+        <v>4992</v>
+      </c>
+      <c r="AA20" s="7">
+        <v>9422</v>
+      </c>
+      <c r="AB20" s="9">
+        <v>19297</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B21" s="15">
         <v>2</v>
       </c>
       <c r="C21" s="7">
-        <v>16006</v>
+        <v>6447</v>
       </c>
       <c r="D21" s="7">
-        <v>20670</v>
+        <v>8128</v>
       </c>
       <c r="E21" s="7">
-        <v>42167</v>
+        <v>15816</v>
       </c>
       <c r="F21" s="8">
-        <v>5398</v>
+        <v>2093</v>
       </c>
       <c r="G21" s="7">
-        <v>9797</v>
+        <v>4070</v>
       </c>
       <c r="H21" s="7">
-        <v>17894</v>
+        <v>8690</v>
       </c>
       <c r="I21" s="8">
-        <v>5008</v>
+        <v>1972</v>
       </c>
       <c r="J21" s="7">
-        <v>9126</v>
+        <v>4062</v>
       </c>
       <c r="K21" s="7">
-        <v>22168</v>
+        <v>11462</v>
       </c>
       <c r="L21" s="8">
-        <v>5476</v>
+        <v>2096</v>
       </c>
       <c r="M21" s="7">
-        <v>11123</v>
+        <v>4619</v>
       </c>
       <c r="N21" s="9">
-        <v>33197</v>
+        <v>16043</v>
+      </c>
+      <c r="P21" s="15">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="7">
+        <v>6318</v>
+      </c>
+      <c r="R21" s="7">
+        <v>10655</v>
+      </c>
+      <c r="S21" s="7">
+        <v>18533</v>
+      </c>
+      <c r="T21" s="8">
+        <v>4727</v>
+      </c>
+      <c r="U21" s="7">
+        <v>9032</v>
+      </c>
+      <c r="V21" s="7">
+        <v>15944</v>
+      </c>
+      <c r="W21" s="8">
+        <v>4758</v>
+      </c>
+      <c r="X21" s="7">
+        <v>8814</v>
+      </c>
+      <c r="Y21" s="7">
+        <v>19142</v>
+      </c>
+      <c r="Z21" s="8">
+        <v>5179</v>
+      </c>
+      <c r="AA21" s="7">
+        <v>10202</v>
+      </c>
+      <c r="AB21" s="9">
+        <v>23759</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B22" s="15">
         <v>5</v>
       </c>
       <c r="C22" s="7">
-        <v>16099</v>
+        <v>6481</v>
       </c>
       <c r="D22" s="7">
-        <v>19141</v>
+        <v>7473</v>
       </c>
       <c r="E22" s="7">
-        <v>34148</v>
+        <v>17725</v>
       </c>
       <c r="F22" s="8">
-        <v>5647</v>
+        <v>2203</v>
       </c>
       <c r="G22" s="7">
-        <v>9454</v>
+        <v>4536</v>
       </c>
       <c r="H22" s="7">
-        <v>20077</v>
+        <v>12876</v>
       </c>
       <c r="I22" s="8">
-        <v>5195</v>
+        <v>2390</v>
       </c>
       <c r="J22" s="7">
-        <v>9719</v>
+        <v>6020</v>
       </c>
       <c r="K22" s="7">
-        <v>33431</v>
+        <v>17678</v>
       </c>
       <c r="L22" s="8">
-        <v>7083</v>
+        <v>2977</v>
       </c>
       <c r="M22" s="7">
-        <v>13213</v>
+        <v>6084</v>
       </c>
       <c r="N22" s="9">
-        <v>49422</v>
+        <v>24936</v>
+      </c>
+      <c r="P22" s="15">
+        <v>5</v>
+      </c>
+      <c r="Q22" s="7">
+        <v>6208</v>
+      </c>
+      <c r="R22" s="7">
+        <v>10905</v>
+      </c>
+      <c r="S22" s="7">
+        <v>24040</v>
+      </c>
+      <c r="T22" s="8">
+        <v>4899</v>
+      </c>
+      <c r="U22" s="7">
+        <v>8378</v>
+      </c>
+      <c r="V22" s="7">
+        <v>15975</v>
+      </c>
+      <c r="W22" s="8">
+        <v>4851</v>
+      </c>
+      <c r="X22" s="7">
+        <v>8237</v>
+      </c>
+      <c r="Y22" s="7">
+        <v>24726</v>
+      </c>
+      <c r="Z22" s="8">
+        <v>5725</v>
+      </c>
+      <c r="AA22" s="7">
+        <v>11669</v>
+      </c>
+      <c r="AB22" s="9">
+        <v>49780</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B23" s="15">
         <v>10</v>
       </c>
       <c r="C23" s="7">
-        <v>16099</v>
+        <v>5622</v>
       </c>
       <c r="D23" s="7">
-        <v>26442</v>
+        <v>9730</v>
       </c>
       <c r="E23" s="7">
-        <v>40280</v>
+        <v>21104</v>
       </c>
       <c r="F23" s="8">
-        <v>5975</v>
+        <v>2410</v>
       </c>
       <c r="G23" s="7">
-        <v>10265</v>
+        <v>5435</v>
       </c>
       <c r="H23" s="7">
-        <v>24492</v>
+        <v>18591</v>
       </c>
       <c r="I23" s="8">
-        <v>5522</v>
+        <v>2908</v>
       </c>
       <c r="J23" s="7">
-        <v>14134</v>
+        <v>8080</v>
       </c>
       <c r="K23" s="7">
-        <v>61183</v>
+        <v>31644</v>
       </c>
       <c r="L23" s="8">
-        <v>9360</v>
+        <v>4160</v>
       </c>
       <c r="M23" s="7">
-        <v>18657</v>
+        <v>8772</v>
       </c>
       <c r="N23" s="9">
-        <v>84241</v>
+        <v>43640</v>
+      </c>
+      <c r="P23" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q23" s="7">
+        <v>6224</v>
+      </c>
+      <c r="R23" s="7">
+        <v>11216</v>
+      </c>
+      <c r="S23" s="7">
+        <v>23634</v>
+      </c>
+      <c r="T23" s="8">
+        <v>5085</v>
+      </c>
+      <c r="U23" s="7">
+        <v>8767</v>
+      </c>
+      <c r="V23" s="7">
+        <v>17721</v>
+      </c>
+      <c r="W23" s="8">
+        <v>4883</v>
+      </c>
+      <c r="X23" s="7">
+        <v>11622</v>
+      </c>
+      <c r="Y23" s="7">
+        <v>36442</v>
+      </c>
+      <c r="Z23" s="8">
+        <v>6708</v>
+      </c>
+      <c r="AA23" s="7">
+        <v>12994</v>
+      </c>
+      <c r="AB23" s="9">
+        <v>64740</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B24" s="15">
         <v>20</v>
       </c>
       <c r="C24" s="7">
-        <v>23306</v>
+        <v>7232</v>
       </c>
       <c r="D24" s="7">
-        <v>35724</v>
+        <v>11965</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="8">
-        <v>6583</v>
+        <v>2861</v>
       </c>
       <c r="G24" s="7">
-        <v>11731</v>
+        <v>7047</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="8">
-        <v>7051</v>
+        <v>4463</v>
       </c>
       <c r="J24" s="7">
-        <v>25038</v>
+        <v>13122</v>
       </c>
       <c r="K24" s="10"/>
       <c r="L24" s="8">
-        <v>14259</v>
+        <v>6646</v>
       </c>
       <c r="M24" s="7">
-        <v>29266</v>
+        <v>14325</v>
       </c>
       <c r="N24" s="11"/>
+      <c r="P24" s="15">
+        <v>20</v>
+      </c>
+      <c r="Q24" s="7">
+        <v>6225</v>
+      </c>
+      <c r="R24" s="7">
+        <v>13432</v>
+      </c>
+      <c r="S24" s="10"/>
+      <c r="T24" s="8">
+        <v>5741</v>
+      </c>
+      <c r="U24" s="7">
+        <v>9079</v>
+      </c>
+      <c r="V24" s="10"/>
+      <c r="W24" s="8">
+        <v>6505</v>
+      </c>
+      <c r="X24" s="7">
+        <v>16271</v>
+      </c>
+      <c r="Y24" s="10"/>
+      <c r="Z24" s="8">
+        <v>9110</v>
+      </c>
+      <c r="AA24" s="7">
+        <v>33493</v>
+      </c>
+      <c r="AB24" s="11"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B25" s="15">
         <v>50</v>
       </c>
       <c r="C25" s="7">
-        <v>24898</v>
+        <v>7575</v>
       </c>
       <c r="D25" s="7">
-        <v>37799</v>
+        <v>14188</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="8">
-        <v>7878</v>
+        <v>4642</v>
       </c>
       <c r="G25" s="7">
-        <v>16193</v>
+        <v>11861</v>
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="8">
-        <v>18003</v>
+        <v>10928</v>
       </c>
       <c r="J25" s="7">
-        <v>47721</v>
+        <v>34427</v>
       </c>
       <c r="K25" s="10"/>
       <c r="L25" s="8">
-        <v>21871</v>
+        <v>10743</v>
       </c>
       <c r="M25" s="7">
-        <v>69967</v>
+        <v>31412</v>
       </c>
       <c r="N25" s="11"/>
+      <c r="P25" s="15">
+        <v>50</v>
+      </c>
+      <c r="Q25" s="7">
+        <v>6224</v>
+      </c>
+      <c r="R25" s="7">
+        <v>14165</v>
+      </c>
+      <c r="S25" s="10"/>
+      <c r="T25" s="8">
+        <v>5928</v>
+      </c>
+      <c r="U25" s="7">
+        <v>10811</v>
+      </c>
+      <c r="V25" s="10"/>
+      <c r="W25" s="8">
+        <v>9392</v>
+      </c>
+      <c r="X25" s="7">
+        <v>26177</v>
+      </c>
+      <c r="Y25" s="10"/>
+      <c r="Z25" s="8">
+        <v>22714</v>
+      </c>
+      <c r="AA25" s="7">
+        <v>50248</v>
+      </c>
+      <c r="AB25" s="11"/>
     </row>
-    <row r="26" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="15">
         <v>100</v>
       </c>
       <c r="C26" s="7">
-        <v>26739</v>
+        <v>8652</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="8">
-        <v>10156</v>
+        <v>7418</v>
       </c>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
       <c r="I26" s="8">
-        <v>38532</v>
+        <v>20605</v>
       </c>
       <c r="J26" s="10"/>
       <c r="K26" s="10"/>
       <c r="L26" s="8">
-        <v>38969</v>
+        <v>20833</v>
       </c>
       <c r="M26" s="10"/>
       <c r="N26" s="11"/>
+      <c r="P26" s="15">
+        <v>100</v>
+      </c>
+      <c r="Q26" s="7">
+        <v>6225</v>
+      </c>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="8">
+        <v>6599</v>
+      </c>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
+      <c r="W26" s="8">
+        <v>15069</v>
+      </c>
+      <c r="X26" s="10"/>
+      <c r="Y26" s="10"/>
+      <c r="Z26" s="8">
+        <v>31029</v>
+      </c>
+      <c r="AA26" s="10"/>
+      <c r="AB26" s="11"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C27" s="4">
-        <f t="shared" ref="C27:N27" si="1">SUM(C20:C26)/86400000</f>
-        <v>1.6112847222222223E-3</v>
+        <f t="shared" ref="C27:N27" si="2">SUM(C20:C26)/86400000</f>
+        <v>5.6208333333333338E-4</v>
       </c>
       <c r="D27" s="4">
-        <f t="shared" si="1"/>
-        <v>1.8584606481481481E-3</v>
-      </c>
-      <c r="E27" s="5">
-        <f t="shared" si="1"/>
-        <v>1.7393055555555556E-3</v>
-      </c>
-      <c r="F27" s="4">
-        <f t="shared" si="1"/>
-        <v>5.4293981481481478E-4</v>
-      </c>
-      <c r="G27" s="4">
-        <f t="shared" si="1"/>
-        <v>7.7531249999999996E-4</v>
-      </c>
-      <c r="H27" s="5">
-        <f t="shared" si="1"/>
-        <v>9.1902777777777772E-4</v>
-      </c>
-      <c r="I27" s="4">
-        <f t="shared" si="1"/>
-        <v>9.7518518518518516E-4</v>
-      </c>
-      <c r="J27" s="4">
-        <f t="shared" si="1"/>
-        <v>1.3285416666666667E-3</v>
-      </c>
-      <c r="K27" s="5">
-        <f t="shared" si="1"/>
-        <v>1.5536805555555555E-3</v>
-      </c>
-      <c r="L27" s="4">
-        <f t="shared" si="1"/>
-        <v>1.182662037037037E-3</v>
-      </c>
-      <c r="M27" s="4">
-        <f t="shared" si="1"/>
-        <v>1.7622337962962962E-3</v>
-      </c>
-      <c r="N27" s="6">
-        <f t="shared" si="1"/>
-        <v>2.2114814814814814E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="18">
-        <f>SUM(C27:E27)</f>
-        <v>5.209050925925926E-3</v>
-      </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="21">
-        <f>SUM(F27:H27)</f>
-        <v>2.2372800925925924E-3</v>
-      </c>
-      <c r="G28" s="19"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="21">
-        <f>SUM(I27:K27)</f>
-        <v>3.8574074074074075E-3</v>
-      </c>
-      <c r="J28" s="19"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="21">
-        <f>SUM(L27:N27)</f>
-        <v>5.156377314814815E-3</v>
-      </c>
-      <c r="M28" s="19"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="17"/>
-    </row>
-    <row r="30" spans="2:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="30"/>
-      <c r="M30" s="30"/>
-      <c r="N30" s="30"/>
-    </row>
-    <row r="31" spans="2:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="23">
-        <v>1</v>
-      </c>
-      <c r="D32" s="24"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="26">
-        <v>100</v>
-      </c>
-      <c r="G32" s="27"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="26">
-        <v>10000</v>
-      </c>
-      <c r="J32" s="27"/>
-      <c r="K32" s="28"/>
-      <c r="L32" s="26">
-        <v>1000000</v>
-      </c>
-      <c r="M32" s="27"/>
-      <c r="N32" s="29"/>
-    </row>
-    <row r="33" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="12">
-        <v>1</v>
-      </c>
-      <c r="D33" s="12">
-        <v>2</v>
-      </c>
-      <c r="E33" s="12">
-        <v>4</v>
-      </c>
-      <c r="F33" s="13">
-        <v>1</v>
-      </c>
-      <c r="G33" s="12">
-        <v>2</v>
-      </c>
-      <c r="H33" s="12">
-        <v>4</v>
-      </c>
-      <c r="I33" s="13">
-        <v>1</v>
-      </c>
-      <c r="J33" s="12">
-        <v>2</v>
-      </c>
-      <c r="K33" s="12">
-        <v>4</v>
-      </c>
-      <c r="L33" s="13">
-        <v>1</v>
-      </c>
-      <c r="M33" s="12">
-        <v>2</v>
-      </c>
-      <c r="N33" s="14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B34" s="15">
-        <v>1</v>
-      </c>
-      <c r="C34" s="7">
-        <v>6555</v>
-      </c>
-      <c r="D34" s="7">
-        <v>8065</v>
-      </c>
-      <c r="E34" s="7">
-        <v>13054</v>
-      </c>
-      <c r="F34" s="8">
-        <v>2385</v>
-      </c>
-      <c r="G34" s="7">
-        <v>3872</v>
-      </c>
-      <c r="H34" s="7">
-        <v>7894</v>
-      </c>
-      <c r="I34" s="8">
-        <v>2354</v>
-      </c>
-      <c r="J34" s="7">
-        <v>3649</v>
-      </c>
-      <c r="K34" s="7">
-        <v>9393</v>
-      </c>
-      <c r="L34" s="8">
-        <v>2397</v>
-      </c>
-      <c r="M34" s="7">
-        <v>4029</v>
-      </c>
-      <c r="N34" s="9">
-        <v>11527</v>
-      </c>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="15">
-        <v>2</v>
-      </c>
-      <c r="C35" s="7">
-        <v>6447</v>
-      </c>
-      <c r="D35" s="7">
-        <v>8128</v>
-      </c>
-      <c r="E35" s="7">
-        <v>15816</v>
-      </c>
-      <c r="F35" s="8">
-        <v>2093</v>
-      </c>
-      <c r="G35" s="7">
-        <v>4070</v>
-      </c>
-      <c r="H35" s="7">
-        <v>8690</v>
-      </c>
-      <c r="I35" s="8">
-        <v>1972</v>
-      </c>
-      <c r="J35" s="7">
-        <v>4062</v>
-      </c>
-      <c r="K35" s="7">
-        <v>11462</v>
-      </c>
-      <c r="L35" s="8">
-        <v>2096</v>
-      </c>
-      <c r="M35" s="7">
-        <v>4619</v>
-      </c>
-      <c r="N35" s="9">
-        <v>16043</v>
-      </c>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B36" s="15">
-        <v>5</v>
-      </c>
-      <c r="C36" s="7">
-        <v>6481</v>
-      </c>
-      <c r="D36" s="7">
-        <v>7473</v>
-      </c>
-      <c r="E36" s="7">
-        <v>17725</v>
-      </c>
-      <c r="F36" s="8">
-        <v>2203</v>
-      </c>
-      <c r="G36" s="7">
-        <v>4536</v>
-      </c>
-      <c r="H36" s="7">
-        <v>12876</v>
-      </c>
-      <c r="I36" s="8">
-        <v>2390</v>
-      </c>
-      <c r="J36" s="7">
-        <v>6020</v>
-      </c>
-      <c r="K36" s="7">
-        <v>17678</v>
-      </c>
-      <c r="L36" s="8">
-        <v>2977</v>
-      </c>
-      <c r="M36" s="7">
-        <v>6084</v>
-      </c>
-      <c r="N36" s="9">
-        <v>24936</v>
-      </c>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="15">
-        <v>10</v>
-      </c>
-      <c r="C37" s="7">
-        <v>5622</v>
-      </c>
-      <c r="D37" s="7">
-        <v>9730</v>
-      </c>
-      <c r="E37" s="7">
-        <v>21104</v>
-      </c>
-      <c r="F37" s="8">
-        <v>2410</v>
-      </c>
-      <c r="G37" s="7">
-        <v>5435</v>
-      </c>
-      <c r="H37" s="7">
-        <v>18591</v>
-      </c>
-      <c r="I37" s="8">
-        <v>2908</v>
-      </c>
-      <c r="J37" s="7">
-        <v>8080</v>
-      </c>
-      <c r="K37" s="7">
-        <v>31644</v>
-      </c>
-      <c r="L37" s="8">
-        <v>4160</v>
-      </c>
-      <c r="M37" s="7">
-        <v>8772</v>
-      </c>
-      <c r="N37" s="9">
-        <v>43640</v>
-      </c>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B38" s="15">
-        <v>20</v>
-      </c>
-      <c r="C38" s="7">
-        <v>7232</v>
-      </c>
-      <c r="D38" s="7">
-        <v>11965</v>
-      </c>
-      <c r="E38" s="10"/>
-      <c r="F38" s="8">
-        <v>2861</v>
-      </c>
-      <c r="G38" s="7">
-        <v>7047</v>
-      </c>
-      <c r="H38" s="10"/>
-      <c r="I38" s="8">
-        <v>4463</v>
-      </c>
-      <c r="J38" s="7">
-        <v>13122</v>
-      </c>
-      <c r="K38" s="10"/>
-      <c r="L38" s="8">
-        <v>6646</v>
-      </c>
-      <c r="M38" s="7">
-        <v>14325</v>
-      </c>
-      <c r="N38" s="11"/>
-    </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B39" s="15">
-        <v>50</v>
-      </c>
-      <c r="C39" s="7">
-        <v>7575</v>
-      </c>
-      <c r="D39" s="7">
-        <v>14188</v>
-      </c>
-      <c r="E39" s="10"/>
-      <c r="F39" s="8">
-        <v>4642</v>
-      </c>
-      <c r="G39" s="7">
-        <v>11861</v>
-      </c>
-      <c r="H39" s="10"/>
-      <c r="I39" s="8">
-        <v>10928</v>
-      </c>
-      <c r="J39" s="7">
-        <v>34427</v>
-      </c>
-      <c r="K39" s="10"/>
-      <c r="L39" s="8">
-        <v>10743</v>
-      </c>
-      <c r="M39" s="7">
-        <v>31412</v>
-      </c>
-      <c r="N39" s="11"/>
-    </row>
-    <row r="40" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="15">
-        <v>100</v>
-      </c>
-      <c r="C40" s="7">
-        <v>8652</v>
-      </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="8">
-        <v>7418</v>
-      </c>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="8">
-        <v>20605</v>
-      </c>
-      <c r="J40" s="10"/>
-      <c r="K40" s="10"/>
-      <c r="L40" s="8">
-        <v>20833</v>
-      </c>
-      <c r="M40" s="10"/>
-      <c r="N40" s="11"/>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B41" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C41" s="4">
-        <f t="shared" ref="C41:N41" si="2">SUM(C34:C40)/86400000</f>
-        <v>5.6208333333333338E-4</v>
-      </c>
-      <c r="D41" s="4">
         <f t="shared" si="2"/>
         <v>6.8922453703703702E-4</v>
       </c>
-      <c r="E41" s="5">
+      <c r="E27" s="5">
         <f t="shared" si="2"/>
         <v>7.8355324074074069E-4</v>
       </c>
-      <c r="F41" s="4">
+      <c r="F27" s="4">
         <f t="shared" si="2"/>
         <v>2.7791666666666665E-4</v>
       </c>
-      <c r="G41" s="4">
+      <c r="G27" s="4">
         <f t="shared" si="2"/>
         <v>4.2616898148148147E-4</v>
       </c>
-      <c r="H41" s="5">
+      <c r="H27" s="5">
         <f t="shared" si="2"/>
         <v>5.561458333333333E-4</v>
       </c>
-      <c r="I41" s="4">
+      <c r="I27" s="4">
         <f t="shared" si="2"/>
         <v>5.2800925925925921E-4</v>
       </c>
-      <c r="J41" s="4">
+      <c r="J27" s="4">
         <f t="shared" si="2"/>
         <v>8.027777777777778E-4</v>
       </c>
-      <c r="K41" s="5">
+      <c r="K27" s="5">
         <f t="shared" si="2"/>
         <v>8.1223379629629625E-4</v>
       </c>
-      <c r="L41" s="4">
+      <c r="L27" s="4">
         <f t="shared" si="2"/>
         <v>5.7699074074074076E-4</v>
       </c>
-      <c r="M41" s="4">
+      <c r="M27" s="4">
         <f t="shared" si="2"/>
         <v>8.0140046296296296E-4</v>
       </c>
-      <c r="N41" s="6">
+      <c r="N27" s="6">
         <f t="shared" si="2"/>
         <v>1.1128009259259259E-3</v>
       </c>
+      <c r="P27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="4">
+        <f t="shared" ref="Q27:AB27" si="3">SUM(Q20:Q26)/86400000</f>
+        <v>5.0537037037037033E-4</v>
+      </c>
+      <c r="R27" s="4">
+        <f t="shared" si="3"/>
+        <v>8.2225694444444447E-4</v>
+      </c>
+      <c r="S27" s="5">
+        <f t="shared" si="3"/>
+        <v>9.7518518518518516E-4</v>
+      </c>
+      <c r="T27" s="4">
+        <f t="shared" si="3"/>
+        <v>4.3604166666666666E-4</v>
+      </c>
+      <c r="U27" s="4">
+        <f t="shared" si="3"/>
+        <v>6.3591435185185181E-4</v>
+      </c>
+      <c r="V27" s="5">
+        <f t="shared" si="3"/>
+        <v>7.5689814814814814E-4</v>
+      </c>
+      <c r="W27" s="4">
+        <f t="shared" si="3"/>
+        <v>5.8067129629629625E-4</v>
+      </c>
+      <c r="X27" s="4">
+        <f t="shared" si="3"/>
+        <v>9.253587962962963E-4</v>
+      </c>
+      <c r="Y27" s="5">
+        <f t="shared" si="3"/>
+        <v>1.1209027777777777E-3</v>
+      </c>
+      <c r="Z27" s="4">
+        <f t="shared" si="3"/>
+        <v>9.8908564814814822E-4</v>
+      </c>
+      <c r="AA27" s="4">
+        <f t="shared" si="3"/>
+        <v>1.4818055555555557E-3</v>
+      </c>
+      <c r="AB27" s="6">
+        <f t="shared" si="3"/>
+        <v>1.8237962962962962E-3</v>
+      </c>
     </row>
-    <row r="42" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="18">
-        <f>SUM(C41:E41)</f>
+    <row r="28" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="26">
+        <f>SUM(C27:E27)</f>
         <v>2.0348611111111114E-3</v>
       </c>
-      <c r="D42" s="19"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="21">
-        <f>SUM(F41:H41)</f>
+      <c r="D28" s="27"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="29">
+        <f>SUM(F27:H27)</f>
         <v>1.2602314814814815E-3</v>
       </c>
-      <c r="G42" s="19"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="21">
-        <f>SUM(I41:K41)</f>
+      <c r="G28" s="27"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="29">
+        <f>SUM(I27:K27)</f>
         <v>2.1430208333333331E-3</v>
       </c>
-      <c r="J42" s="19"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="21">
-        <f>SUM(L41:N41)</f>
+      <c r="J28" s="27"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="29">
+        <f>SUM(L27:N27)</f>
         <v>2.4911921296296297E-3</v>
       </c>
-      <c r="M42" s="19"/>
-      <c r="N42" s="22"/>
+      <c r="M28" s="27"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="26">
+        <f>SUM(Q27:S27)</f>
+        <v>2.3028125000000002E-3</v>
+      </c>
+      <c r="R28" s="27"/>
+      <c r="S28" s="28"/>
+      <c r="T28" s="29">
+        <f>SUM(T27:V27)</f>
+        <v>1.8288541666666666E-3</v>
+      </c>
+      <c r="U28" s="27"/>
+      <c r="V28" s="28"/>
+      <c r="W28" s="29">
+        <f>SUM(W27:Y27)</f>
+        <v>2.6269328703703706E-3</v>
+      </c>
+      <c r="X28" s="27"/>
+      <c r="Y28" s="28"/>
+      <c r="Z28" s="29">
+        <f>SUM(Z27:AB27)</f>
+        <v>4.2946874999999999E-3</v>
+      </c>
+      <c r="AA28" s="27"/>
+      <c r="AB28" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B30:N30"/>
-    <mergeCell ref="B16:N16"/>
+  <mergeCells count="36">
+    <mergeCell ref="Q28:S28"/>
+    <mergeCell ref="T28:V28"/>
+    <mergeCell ref="W28:Y28"/>
+    <mergeCell ref="Z28:AB28"/>
+    <mergeCell ref="Z14:AB14"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="T4:V4"/>
+    <mergeCell ref="P16:AB16"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="T18:V18"/>
+    <mergeCell ref="W18:Y18"/>
+    <mergeCell ref="Z18:AB18"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:H18"/>
     <mergeCell ref="I18:K18"/>
     <mergeCell ref="L18:N18"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="L32:N32"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="L42:N42"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="L28:N28"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B16:N16"/>
+    <mergeCell ref="P2:AB2"/>
+    <mergeCell ref="W4:Y4"/>
+    <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="I4:K4"/>
@@ -1991,26 +2377,11 @@
     <mergeCell ref="F14:H14"/>
     <mergeCell ref="I14:K14"/>
     <mergeCell ref="L14:N14"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="L28:N28"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="T14:V14"/>
+    <mergeCell ref="W14:Y14"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:N12">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="num" val="1000"/>
-        <cfvo type="num" val="10000"/>
-        <cfvo type="num" val="30000"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34:N40">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="num" val="1000"/>
@@ -2023,7 +2394,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:N26">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="num" val="1000"/>
         <cfvo type="num" val="10000"/>
@@ -2034,8 +2405,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:N28">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="Q6:AB12">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="num" val="1000"/>
+        <cfvo type="num" val="10000"/>
+        <cfvo type="num" val="30000"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q14:AB14">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="1E-3"/>
         <cfvo type="num" val="2.5000000000000001E-3"/>
@@ -2047,7 +2430,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:N14">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="1E-3"/>
         <cfvo type="num" val="2.5000000000000001E-3"/>
@@ -2058,7 +2441,31 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C42:N42">
+  <conditionalFormatting sqref="C28:N28">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="1E-3"/>
+        <cfvo type="num" val="2.5000000000000001E-3"/>
+        <cfvo type="num" val="4.0000000000000001E-3"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q20:AB26">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="1000"/>
+        <cfvo type="num" val="10000"/>
+        <cfvo type="num" val="30000"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q28:AB28">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="1E-3"/>
@@ -2073,7 +2480,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C13:N13 C27:N27 C41:N41" formulaRange="1"/>
+    <ignoredError sqref="C13:N13 Q27:AB27 Q13:AB13 C27:N28" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added optimized "for" cycle mode to Delphi version, updated charts (also added % comparison)
</commit_message>
<xml_diff>
--- a/Results/StringBuilder.xlsx
+++ b/Results/StringBuilder.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
   <si>
     <t>Repeat</t>
   </si>
@@ -39,13 +39,20 @@
   <si>
     <t>.NET 3.5 (StringBuilder)</t>
   </si>
+  <si>
+    <t>Delphi XE3 (+, for)</t>
+  </si>
+  <si>
+    <t>.NET 4.5 (StringBuilder) vs Delphi XE3 (+, for)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m:ss.00"/>
+    <numFmt numFmtId="166" formatCode="\+0%;\−0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -101,7 +108,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -349,12 +356,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -375,13 +433,11 @@
     <xf numFmtId="3" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -391,11 +447,31 @@
     <xf numFmtId="3" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -698,7 +774,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AB28"/>
+  <dimension ref="B2:AB42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -708,36 +784,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:28" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="P2" s="18" t="s">
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="P2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="18"/>
-      <c r="X2" s="18"/>
-      <c r="Y2" s="18"/>
-      <c r="Z2" s="18"/>
-      <c r="AA2" s="18"/>
-      <c r="AB2" s="18"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="29"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="29"/>
+      <c r="Z2" s="29"/>
+      <c r="AA2" s="29"/>
+      <c r="AB2" s="29"/>
     </row>
     <row r="3" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
@@ -749,21 +825,21 @@
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="25"/>
-      <c r="F4" s="19">
+      <c r="F4" s="26">
         <v>100</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="19">
+      <c r="G4" s="27"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="26">
         <v>10000</v>
       </c>
-      <c r="J4" s="20"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="19">
+      <c r="J4" s="27"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="26">
         <v>1000000</v>
       </c>
-      <c r="M4" s="20"/>
-      <c r="N4" s="22"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="30"/>
       <c r="P4" s="1" t="s">
         <v>0</v>
       </c>
@@ -772,21 +848,21 @@
       </c>
       <c r="R4" s="24"/>
       <c r="S4" s="25"/>
-      <c r="T4" s="19">
+      <c r="T4" s="26">
         <v>100</v>
       </c>
-      <c r="U4" s="20"/>
-      <c r="V4" s="21"/>
-      <c r="W4" s="19">
+      <c r="U4" s="27"/>
+      <c r="V4" s="28"/>
+      <c r="W4" s="26">
         <v>10000</v>
       </c>
-      <c r="X4" s="20"/>
-      <c r="Y4" s="21"/>
-      <c r="Z4" s="19">
+      <c r="X4" s="27"/>
+      <c r="Y4" s="28"/>
+      <c r="Z4" s="26">
         <v>1000000</v>
       </c>
-      <c r="AA4" s="20"/>
-      <c r="AB4" s="22"/>
+      <c r="AA4" s="27"/>
+      <c r="AB4" s="30"/>
     </row>
     <row r="5" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="16" t="s">
@@ -1472,89 +1548,89 @@
       <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="18">
         <f>SUM(C13:E13)</f>
         <v>2.2150115740740741E-3</v>
       </c>
-      <c r="D14" s="27"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="29">
+      <c r="D14" s="19"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21">
         <f>SUM(F13:H13)</f>
         <v>9.4211805555555542E-4</v>
       </c>
-      <c r="G14" s="27"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="29">
+      <c r="G14" s="19"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="21">
         <f>SUM(I13:K13)</f>
         <v>1.7703935185185186E-3</v>
       </c>
-      <c r="J14" s="27"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="29">
+      <c r="J14" s="19"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="21">
         <f>SUM(L13:N13)</f>
         <v>3.5719675925925927E-3</v>
       </c>
-      <c r="M14" s="27"/>
-      <c r="N14" s="30"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="22"/>
       <c r="P14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q14" s="26">
+      <c r="Q14" s="18">
         <f>SUM(Q13:S13)</f>
         <v>5.209050925925926E-3</v>
       </c>
-      <c r="R14" s="27"/>
-      <c r="S14" s="28"/>
-      <c r="T14" s="29">
+      <c r="R14" s="19"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="21">
         <f>SUM(T13:V13)</f>
         <v>2.2372800925925924E-3</v>
       </c>
-      <c r="U14" s="27"/>
-      <c r="V14" s="28"/>
-      <c r="W14" s="29">
+      <c r="U14" s="19"/>
+      <c r="V14" s="20"/>
+      <c r="W14" s="21">
         <f>SUM(W13:Y13)</f>
         <v>3.8574074074074075E-3</v>
       </c>
-      <c r="X14" s="27"/>
-      <c r="Y14" s="28"/>
-      <c r="Z14" s="29">
+      <c r="X14" s="19"/>
+      <c r="Y14" s="20"/>
+      <c r="Z14" s="21">
         <f>SUM(Z13:AB13)</f>
         <v>5.156377314814815E-3</v>
       </c>
-      <c r="AA14" s="27"/>
-      <c r="AB14" s="30"/>
+      <c r="AA14" s="19"/>
+      <c r="AB14" s="22"/>
     </row>
     <row r="16" spans="2:28" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="P16" s="18" t="s">
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+      <c r="P16" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="18"/>
-      <c r="U16" s="18"/>
-      <c r="V16" s="18"/>
-      <c r="W16" s="18"/>
-      <c r="X16" s="18"/>
-      <c r="Y16" s="18"/>
-      <c r="Z16" s="18"/>
-      <c r="AA16" s="18"/>
-      <c r="AB16" s="18"/>
+      <c r="Q16" s="29"/>
+      <c r="R16" s="29"/>
+      <c r="S16" s="29"/>
+      <c r="T16" s="29"/>
+      <c r="U16" s="29"/>
+      <c r="V16" s="29"/>
+      <c r="W16" s="29"/>
+      <c r="X16" s="29"/>
+      <c r="Y16" s="29"/>
+      <c r="Z16" s="29"/>
+      <c r="AA16" s="29"/>
+      <c r="AB16" s="29"/>
     </row>
     <row r="17" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:28" x14ac:dyDescent="0.25">
@@ -1566,21 +1642,21 @@
       </c>
       <c r="D18" s="24"/>
       <c r="E18" s="25"/>
-      <c r="F18" s="19">
+      <c r="F18" s="26">
         <v>100</v>
       </c>
-      <c r="G18" s="20"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="19">
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="26">
         <v>10000</v>
       </c>
-      <c r="J18" s="20"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="19">
+      <c r="J18" s="27"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="26">
         <v>1000000</v>
       </c>
-      <c r="M18" s="20"/>
-      <c r="N18" s="22"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="30"/>
       <c r="P18" s="1" t="s">
         <v>0</v>
       </c>
@@ -1589,21 +1665,21 @@
       </c>
       <c r="R18" s="24"/>
       <c r="S18" s="25"/>
-      <c r="T18" s="19">
+      <c r="T18" s="26">
         <v>100</v>
       </c>
-      <c r="U18" s="20"/>
-      <c r="V18" s="21"/>
-      <c r="W18" s="19">
+      <c r="U18" s="27"/>
+      <c r="V18" s="28"/>
+      <c r="W18" s="26">
         <v>10000</v>
       </c>
-      <c r="X18" s="20"/>
-      <c r="Y18" s="21"/>
-      <c r="Z18" s="19">
+      <c r="X18" s="27"/>
+      <c r="Y18" s="28"/>
+      <c r="Z18" s="26">
         <v>1000000</v>
       </c>
-      <c r="AA18" s="20"/>
-      <c r="AB18" s="22"/>
+      <c r="AA18" s="27"/>
+      <c r="AB18" s="30"/>
     </row>
     <row r="19" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="16" t="s">
@@ -2289,81 +2365,964 @@
       <c r="B28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="26">
+      <c r="C28" s="18">
         <f>SUM(C27:E27)</f>
         <v>2.0348611111111114E-3</v>
       </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="29">
+      <c r="D28" s="19"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="21">
         <f>SUM(F27:H27)</f>
         <v>1.2602314814814815E-3</v>
       </c>
-      <c r="G28" s="27"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="29">
+      <c r="G28" s="19"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="21">
         <f>SUM(I27:K27)</f>
         <v>2.1430208333333331E-3</v>
       </c>
-      <c r="J28" s="27"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="29">
+      <c r="J28" s="19"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="21">
         <f>SUM(L27:N27)</f>
         <v>2.4911921296296297E-3</v>
       </c>
-      <c r="M28" s="27"/>
-      <c r="N28" s="30"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="22"/>
       <c r="O28" s="17"/>
       <c r="P28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q28" s="26">
+      <c r="Q28" s="18">
         <f>SUM(Q27:S27)</f>
         <v>2.3028125000000002E-3</v>
       </c>
-      <c r="R28" s="27"/>
-      <c r="S28" s="28"/>
-      <c r="T28" s="29">
+      <c r="R28" s="19"/>
+      <c r="S28" s="20"/>
+      <c r="T28" s="21">
         <f>SUM(T27:V27)</f>
         <v>1.8288541666666666E-3</v>
       </c>
-      <c r="U28" s="27"/>
-      <c r="V28" s="28"/>
-      <c r="W28" s="29">
+      <c r="U28" s="19"/>
+      <c r="V28" s="20"/>
+      <c r="W28" s="21">
         <f>SUM(W27:Y27)</f>
         <v>2.6269328703703706E-3</v>
       </c>
-      <c r="X28" s="27"/>
-      <c r="Y28" s="28"/>
-      <c r="Z28" s="29">
+      <c r="X28" s="19"/>
+      <c r="Y28" s="20"/>
+      <c r="Z28" s="21">
         <f>SUM(Z27:AB27)</f>
         <v>4.2946874999999999E-3</v>
       </c>
-      <c r="AA28" s="27"/>
-      <c r="AB28" s="30"/>
+      <c r="AA28" s="19"/>
+      <c r="AB28" s="22"/>
+    </row>
+    <row r="30" spans="2:28" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="29"/>
+      <c r="P30" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q30" s="29"/>
+      <c r="R30" s="29"/>
+      <c r="S30" s="29"/>
+      <c r="T30" s="29"/>
+      <c r="U30" s="29"/>
+      <c r="V30" s="29"/>
+      <c r="W30" s="29"/>
+      <c r="X30" s="29"/>
+      <c r="Y30" s="29"/>
+      <c r="Z30" s="29"/>
+      <c r="AA30" s="29"/>
+      <c r="AB30" s="29"/>
+    </row>
+    <row r="31" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="24">
+        <v>1</v>
+      </c>
+      <c r="D32" s="24"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="26">
+        <v>100</v>
+      </c>
+      <c r="G32" s="27"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="26">
+        <v>10000</v>
+      </c>
+      <c r="J32" s="27"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="26">
+        <v>1000000</v>
+      </c>
+      <c r="M32" s="27"/>
+      <c r="N32" s="30"/>
+      <c r="P32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="23">
+        <v>1</v>
+      </c>
+      <c r="R32" s="24"/>
+      <c r="S32" s="25"/>
+      <c r="T32" s="26">
+        <v>100</v>
+      </c>
+      <c r="U32" s="27"/>
+      <c r="V32" s="28"/>
+      <c r="W32" s="26">
+        <v>10000</v>
+      </c>
+      <c r="X32" s="27"/>
+      <c r="Y32" s="28"/>
+      <c r="Z32" s="26">
+        <v>1000000</v>
+      </c>
+      <c r="AA32" s="27"/>
+      <c r="AB32" s="30"/>
+    </row>
+    <row r="33" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="31">
+        <v>1</v>
+      </c>
+      <c r="D33" s="31">
+        <v>2</v>
+      </c>
+      <c r="E33" s="31">
+        <v>4</v>
+      </c>
+      <c r="F33" s="13">
+        <v>1</v>
+      </c>
+      <c r="G33" s="12">
+        <v>2</v>
+      </c>
+      <c r="H33" s="12">
+        <v>4</v>
+      </c>
+      <c r="I33" s="13">
+        <v>1</v>
+      </c>
+      <c r="J33" s="12">
+        <v>2</v>
+      </c>
+      <c r="K33" s="12">
+        <v>4</v>
+      </c>
+      <c r="L33" s="13">
+        <v>1</v>
+      </c>
+      <c r="M33" s="12">
+        <v>2</v>
+      </c>
+      <c r="N33" s="14">
+        <v>4</v>
+      </c>
+      <c r="P33" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q33" s="12">
+        <v>1</v>
+      </c>
+      <c r="R33" s="12">
+        <v>2</v>
+      </c>
+      <c r="S33" s="12">
+        <v>4</v>
+      </c>
+      <c r="T33" s="13">
+        <v>1</v>
+      </c>
+      <c r="U33" s="12">
+        <v>2</v>
+      </c>
+      <c r="V33" s="12">
+        <v>4</v>
+      </c>
+      <c r="W33" s="13">
+        <v>1</v>
+      </c>
+      <c r="X33" s="12">
+        <v>2</v>
+      </c>
+      <c r="Y33" s="12">
+        <v>4</v>
+      </c>
+      <c r="Z33" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA33" s="12">
+        <v>2</v>
+      </c>
+      <c r="AB33" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B34" s="15">
+        <v>1</v>
+      </c>
+      <c r="C34" s="32">
+        <f>(C6-Q34)/C6</f>
+        <v>0.3179230243680255</v>
+      </c>
+      <c r="D34" s="32">
+        <f t="shared" ref="D34:N39" si="4">(D6-R34)/D6</f>
+        <v>-4.2989548412541906E-2</v>
+      </c>
+      <c r="E34" s="33">
+        <f t="shared" si="4"/>
+        <v>0.29356410687279449</v>
+      </c>
+      <c r="F34" s="32">
+        <f>(F6-T34)/F6</f>
+        <v>-0.58810068649885583</v>
+      </c>
+      <c r="G34" s="32">
+        <f t="shared" ref="G34:G39" si="5">(G6-U34)/G6</f>
+        <v>-1.5830869308101716</v>
+      </c>
+      <c r="H34" s="33">
+        <f t="shared" ref="H34:H37" si="6">(H6-V34)/H6</f>
+        <v>-0.74824541544034417</v>
+      </c>
+      <c r="I34" s="32">
+        <f>(I6-W34)/I6</f>
+        <v>-1.0771558245083208</v>
+      </c>
+      <c r="J34" s="32">
+        <f t="shared" ref="J34:J39" si="7">(J6-X34)/J6</f>
+        <v>-2.2259013980868287</v>
+      </c>
+      <c r="K34" s="33">
+        <f t="shared" ref="K34:K37" si="8">(K6-Y34)/K6</f>
+        <v>-0.69337694194603439</v>
+      </c>
+      <c r="L34" s="32">
+        <f>(L6-Z34)/L6</f>
+        <v>-1.1898395721925135</v>
+      </c>
+      <c r="M34" s="32">
+        <f t="shared" ref="M34:M39" si="9">(M6-AA34)/M6</f>
+        <v>-1.8508002065049045</v>
+      </c>
+      <c r="N34" s="44">
+        <f t="shared" ref="N34:N37" si="10">(N6-AB34)/N6</f>
+        <v>-0.30935414545865852</v>
+      </c>
+      <c r="P34" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="7">
+        <v>2995</v>
+      </c>
+      <c r="R34" s="7">
+        <v>5289</v>
+      </c>
+      <c r="S34" s="7">
+        <v>8408</v>
+      </c>
+      <c r="T34" s="8">
+        <v>1388</v>
+      </c>
+      <c r="U34" s="7">
+        <v>4368</v>
+      </c>
+      <c r="V34" s="7">
+        <v>7722</v>
+      </c>
+      <c r="W34" s="8">
+        <v>1373</v>
+      </c>
+      <c r="X34" s="7">
+        <v>4384</v>
+      </c>
+      <c r="Y34" s="7">
+        <v>8284</v>
+      </c>
+      <c r="Z34" s="8">
+        <v>1638</v>
+      </c>
+      <c r="AA34" s="7">
+        <v>5522</v>
+      </c>
+      <c r="AB34" s="9">
+        <v>11576</v>
+      </c>
+    </row>
+    <row r="35" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B35" s="15">
+        <v>2</v>
+      </c>
+      <c r="C35" s="34">
+        <f t="shared" ref="C35:C40" si="11">(C7-Q35)/C7</f>
+        <v>0.3428886438809261</v>
+      </c>
+      <c r="D35" s="34">
+        <f t="shared" si="4"/>
+        <v>-1.6898235073225685E-3</v>
+      </c>
+      <c r="E35" s="35">
+        <f t="shared" si="4"/>
+        <v>0.47187481821883542</v>
+      </c>
+      <c r="F35" s="34">
+        <f t="shared" ref="F35:F40" si="12">(F7-T35)/F7</f>
+        <v>-0.27839851024208567</v>
+      </c>
+      <c r="G35" s="34">
+        <f t="shared" si="5"/>
+        <v>-0.99642058165548097</v>
+      </c>
+      <c r="H35" s="35">
+        <f t="shared" si="6"/>
+        <v>-0.32710592160133445</v>
+      </c>
+      <c r="I35" s="34">
+        <f t="shared" ref="I35:I40" si="13">(I7-W35)/I7</f>
+        <v>-0.65821256038647347</v>
+      </c>
+      <c r="J35" s="34">
+        <f t="shared" si="7"/>
+        <v>-0.98301973382285457</v>
+      </c>
+      <c r="K35" s="35">
+        <f t="shared" si="8"/>
+        <v>-0.43633276740237692</v>
+      </c>
+      <c r="L35" s="34">
+        <f t="shared" ref="L35:L40" si="14">(L7-Z35)/L7</f>
+        <v>-0.55791335101679929</v>
+      </c>
+      <c r="M35" s="34">
+        <f t="shared" si="9"/>
+        <v>-0.93728222996515675</v>
+      </c>
+      <c r="N35" s="45">
+        <f t="shared" si="10"/>
+        <v>-3.096153846153846E-2</v>
+      </c>
+      <c r="P35" s="15">
+        <v>2</v>
+      </c>
+      <c r="Q35" s="7">
+        <v>2980</v>
+      </c>
+      <c r="R35" s="7">
+        <v>5335</v>
+      </c>
+      <c r="S35" s="7">
+        <v>9079</v>
+      </c>
+      <c r="T35" s="8">
+        <v>1373</v>
+      </c>
+      <c r="U35" s="7">
+        <v>4462</v>
+      </c>
+      <c r="V35" s="7">
+        <v>7956</v>
+      </c>
+      <c r="W35" s="8">
+        <v>1373</v>
+      </c>
+      <c r="X35" s="7">
+        <v>4321</v>
+      </c>
+      <c r="Y35" s="7">
+        <v>10998</v>
+      </c>
+      <c r="Z35" s="8">
+        <v>1762</v>
+      </c>
+      <c r="AA35" s="7">
+        <v>6116</v>
+      </c>
+      <c r="AB35" s="9">
+        <v>16083</v>
+      </c>
+    </row>
+    <row r="36" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B36" s="15">
+        <v>5</v>
+      </c>
+      <c r="C36" s="34">
+        <f t="shared" si="11"/>
+        <v>0.35990596281256682</v>
+      </c>
+      <c r="D36" s="34">
+        <f t="shared" si="4"/>
+        <v>6.8545697131420946E-2</v>
+      </c>
+      <c r="E36" s="35">
+        <f t="shared" si="4"/>
+        <v>0.22706736382557491</v>
+      </c>
+      <c r="F36" s="34">
+        <f t="shared" si="12"/>
+        <v>1.0464355788096796E-2</v>
+      </c>
+      <c r="G36" s="34">
+        <f t="shared" si="5"/>
+        <v>1.098556183301946E-2</v>
+      </c>
+      <c r="H36" s="35">
+        <f t="shared" si="6"/>
+        <v>0.24069863579991732</v>
+      </c>
+      <c r="I36" s="34">
+        <f t="shared" si="13"/>
+        <v>3.2666666666666663E-2</v>
+      </c>
+      <c r="J36" s="34">
+        <f t="shared" si="7"/>
+        <v>0.18325661680092059</v>
+      </c>
+      <c r="K36" s="35">
+        <f t="shared" si="8"/>
+        <v>4.1465822637783846E-2</v>
+      </c>
+      <c r="L36" s="34">
+        <f t="shared" si="14"/>
+        <v>-1.1175681716584712E-2</v>
+      </c>
+      <c r="M36" s="34">
+        <f t="shared" si="9"/>
+        <v>1.8323820967257435E-2</v>
+      </c>
+      <c r="N36" s="45">
+        <f t="shared" si="10"/>
+        <v>-0.15332476973953921</v>
+      </c>
+      <c r="P36" s="15">
+        <v>5</v>
+      </c>
+      <c r="Q36" s="7">
+        <v>2995</v>
+      </c>
+      <c r="R36" s="7">
+        <v>5585</v>
+      </c>
+      <c r="S36" s="7">
+        <v>15226</v>
+      </c>
+      <c r="T36" s="8">
+        <v>1513</v>
+      </c>
+      <c r="U36" s="7">
+        <v>3151</v>
+      </c>
+      <c r="V36" s="7">
+        <v>7347</v>
+      </c>
+      <c r="W36" s="8">
+        <v>1451</v>
+      </c>
+      <c r="X36" s="7">
+        <v>2839</v>
+      </c>
+      <c r="Y36" s="7">
+        <v>16505</v>
+      </c>
+      <c r="Z36" s="8">
+        <v>2262</v>
+      </c>
+      <c r="AA36" s="7">
+        <v>6536</v>
+      </c>
+      <c r="AB36" s="9">
+        <v>42199</v>
+      </c>
+    </row>
+    <row r="37" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B37" s="15">
+        <v>10</v>
+      </c>
+      <c r="C37" s="34">
+        <f t="shared" si="11"/>
+        <v>0.41396263520157328</v>
+      </c>
+      <c r="D37" s="34">
+        <f t="shared" si="4"/>
+        <v>0.46165784188424319</v>
+      </c>
+      <c r="E37" s="35">
+        <f t="shared" si="4"/>
+        <v>0.4032172457436819</v>
+      </c>
+      <c r="F37" s="34">
+        <f t="shared" si="12"/>
+        <v>6.5217391304347824E-2</v>
+      </c>
+      <c r="G37" s="34">
+        <f t="shared" si="5"/>
+        <v>0.1248780487804878</v>
+      </c>
+      <c r="H37" s="35">
+        <f t="shared" si="6"/>
+        <v>0.36178316992311488</v>
+      </c>
+      <c r="I37" s="34">
+        <f t="shared" si="13"/>
+        <v>0.28557504873294348</v>
+      </c>
+      <c r="J37" s="34">
+        <f t="shared" si="7"/>
+        <v>-0.18228669593433861</v>
+      </c>
+      <c r="K37" s="35">
+        <f t="shared" si="8"/>
+        <v>0.2885982512199351</v>
+      </c>
+      <c r="L37" s="34">
+        <f t="shared" si="14"/>
+        <v>0.10369955156950672</v>
+      </c>
+      <c r="M37" s="34">
+        <f t="shared" si="9"/>
+        <v>0.3655905054361358</v>
+      </c>
+      <c r="N37" s="45">
+        <f t="shared" si="10"/>
+        <v>0.18936658549556357</v>
+      </c>
+      <c r="P37" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q37" s="7">
+        <v>2980</v>
+      </c>
+      <c r="R37" s="7">
+        <v>5897</v>
+      </c>
+      <c r="S37" s="7">
+        <v>14617</v>
+      </c>
+      <c r="T37" s="8">
+        <v>1763</v>
+      </c>
+      <c r="U37" s="7">
+        <v>3588</v>
+      </c>
+      <c r="V37" s="7">
+        <v>9048</v>
+      </c>
+      <c r="W37" s="8">
+        <v>1466</v>
+      </c>
+      <c r="X37" s="7">
+        <v>6194</v>
+      </c>
+      <c r="Y37" s="7">
+        <v>28720</v>
+      </c>
+      <c r="Z37" s="8">
+        <v>3198</v>
+      </c>
+      <c r="AA37" s="7">
+        <v>7644</v>
+      </c>
+      <c r="AB37" s="9">
+        <v>57923</v>
+      </c>
+    </row>
+    <row r="38" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B38" s="15">
+        <v>20</v>
+      </c>
+      <c r="C38" s="34">
+        <f t="shared" si="11"/>
+        <v>0.6892116182572614</v>
+      </c>
+      <c r="D38" s="34">
+        <f t="shared" si="4"/>
+        <v>0.50508329250367467</v>
+      </c>
+      <c r="E38" s="36"/>
+      <c r="F38" s="34">
+        <f t="shared" si="12"/>
+        <v>1.6998341625207296E-2</v>
+      </c>
+      <c r="G38" s="34">
+        <f t="shared" si="5"/>
+        <v>0.29020801623541348</v>
+      </c>
+      <c r="H38" s="36"/>
+      <c r="I38" s="34">
+        <f t="shared" si="13"/>
+        <v>4.4314108830237862E-2</v>
+      </c>
+      <c r="J38" s="34">
+        <f t="shared" si="7"/>
+        <v>-0.22203776717161236</v>
+      </c>
+      <c r="K38" s="36"/>
+      <c r="L38" s="34">
+        <f t="shared" si="14"/>
+        <v>0.25725077566437338</v>
+      </c>
+      <c r="M38" s="34">
+        <f t="shared" si="9"/>
+        <v>-0.25648291258801303</v>
+      </c>
+      <c r="N38" s="46"/>
+      <c r="P38" s="15">
+        <v>20</v>
+      </c>
+      <c r="Q38" s="7">
+        <v>2996</v>
+      </c>
+      <c r="R38" s="7">
+        <v>8081</v>
+      </c>
+      <c r="S38" s="10"/>
+      <c r="T38" s="8">
+        <v>2371</v>
+      </c>
+      <c r="U38" s="7">
+        <v>4197</v>
+      </c>
+      <c r="V38" s="10"/>
+      <c r="W38" s="8">
+        <v>2933</v>
+      </c>
+      <c r="X38" s="7">
+        <v>11778</v>
+      </c>
+      <c r="Y38" s="10"/>
+      <c r="Z38" s="8">
+        <v>5506</v>
+      </c>
+      <c r="AA38" s="7">
+        <v>29266</v>
+      </c>
+      <c r="AB38" s="11"/>
+    </row>
+    <row r="39" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B39" s="15">
+        <v>50</v>
+      </c>
+      <c r="C39" s="34">
+        <f t="shared" si="11"/>
+        <v>0.7358105711245122</v>
+      </c>
+      <c r="D39" s="34">
+        <f t="shared" si="4"/>
+        <v>0.57579245192538242</v>
+      </c>
+      <c r="E39" s="36"/>
+      <c r="F39" s="34">
+        <f t="shared" si="12"/>
+        <v>0.35880167208546215</v>
+      </c>
+      <c r="G39" s="34">
+        <f t="shared" si="5"/>
+        <v>0.43546441495778043</v>
+      </c>
+      <c r="H39" s="36"/>
+      <c r="I39" s="34">
+        <f t="shared" si="13"/>
+        <v>0.13495424122387653</v>
+      </c>
+      <c r="J39" s="34">
+        <f t="shared" si="7"/>
+        <v>0.22059927649989761</v>
+      </c>
+      <c r="K39" s="36"/>
+      <c r="L39" s="34">
+        <f t="shared" si="14"/>
+        <v>-9.2215439468424185E-2</v>
+      </c>
+      <c r="M39" s="34">
+        <f t="shared" si="9"/>
+        <v>0.17735367200441746</v>
+      </c>
+      <c r="N39" s="46"/>
+      <c r="P39" s="15">
+        <v>50</v>
+      </c>
+      <c r="Q39" s="7">
+        <v>2979</v>
+      </c>
+      <c r="R39" s="7">
+        <v>8846</v>
+      </c>
+      <c r="S39" s="10"/>
+      <c r="T39" s="8">
+        <v>2761</v>
+      </c>
+      <c r="U39" s="7">
+        <v>6084</v>
+      </c>
+      <c r="V39" s="10"/>
+      <c r="W39" s="8">
+        <v>6333</v>
+      </c>
+      <c r="X39" s="7">
+        <v>22838</v>
+      </c>
+      <c r="Y39" s="10"/>
+      <c r="Z39" s="8">
+        <v>20218</v>
+      </c>
+      <c r="AA39" s="7">
+        <v>47674</v>
+      </c>
+      <c r="AB39" s="11"/>
+    </row>
+    <row r="40" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="15">
+        <v>100</v>
+      </c>
+      <c r="C40" s="39">
+        <f t="shared" si="11"/>
+        <v>0.78542771170654824</v>
+      </c>
+      <c r="D40" s="37"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="39">
+        <f t="shared" si="12"/>
+        <v>0.51349461613760317</v>
+      </c>
+      <c r="G40" s="37"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="39">
+        <f t="shared" si="13"/>
+        <v>0.23149577134391011</v>
+      </c>
+      <c r="J40" s="37"/>
+      <c r="K40" s="38"/>
+      <c r="L40" s="39">
+        <f t="shared" si="14"/>
+        <v>0.20546410181158453</v>
+      </c>
+      <c r="M40" s="37"/>
+      <c r="N40" s="47"/>
+      <c r="P40" s="15">
+        <v>100</v>
+      </c>
+      <c r="Q40" s="7">
+        <v>2995</v>
+      </c>
+      <c r="R40" s="10"/>
+      <c r="S40" s="10"/>
+      <c r="T40" s="8">
+        <v>3479</v>
+      </c>
+      <c r="U40" s="10"/>
+      <c r="V40" s="10"/>
+      <c r="W40" s="8">
+        <v>12449</v>
+      </c>
+      <c r="X40" s="10"/>
+      <c r="Y40" s="10"/>
+      <c r="Z40" s="8">
+        <v>29780</v>
+      </c>
+      <c r="AA40" s="10"/>
+      <c r="AB40" s="11"/>
+    </row>
+    <row r="41" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="40">
+        <f>(SUM(C6:C12)-SUM(Q34:Q40))/SUM(C6:C12)</f>
+        <v>0.60943917556567839</v>
+      </c>
+      <c r="D41" s="40">
+        <f t="shared" ref="D41:N41" si="15">(SUM(D6:D12)-SUM(R34:R40))/SUM(D6:D12)</f>
+        <v>0.39509980163649888</v>
+      </c>
+      <c r="E41" s="41">
+        <f t="shared" si="15"/>
+        <v>0.35416524527529508</v>
+      </c>
+      <c r="F41" s="40">
+        <f t="shared" si="15"/>
+        <v>0.23835274542429286</v>
+      </c>
+      <c r="G41" s="40">
+        <f t="shared" si="15"/>
+        <v>7.3543115188875352E-2</v>
+      </c>
+      <c r="H41" s="41">
+        <f t="shared" si="15"/>
+        <v>6.397198307310667E-2</v>
+      </c>
+      <c r="I41" s="40">
+        <f t="shared" si="15"/>
+        <v>0.13442933923490358</v>
+      </c>
+      <c r="J41" s="40">
+        <f t="shared" si="15"/>
+        <v>-2.267888187838181E-2</v>
+      </c>
+      <c r="K41" s="41">
+        <f t="shared" si="15"/>
+        <v>8.0297694577909584E-2</v>
+      </c>
+      <c r="L41" s="40">
+        <f t="shared" si="15"/>
+        <v>9.4599727102645984E-2</v>
+      </c>
+      <c r="M41" s="40">
+        <f t="shared" si="15"/>
+        <v>2.1771621685944119E-2</v>
+      </c>
+      <c r="N41" s="48">
+        <f t="shared" si="15"/>
+        <v>3.5498626249207452E-2</v>
+      </c>
+      <c r="P41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q41" s="4">
+        <f t="shared" ref="Q41:AB41" si="16">SUM(Q34:Q40)/86400000</f>
+        <v>2.4212962962962963E-4</v>
+      </c>
+      <c r="R41" s="4">
+        <f t="shared" si="16"/>
+        <v>4.5177083333333332E-4</v>
+      </c>
+      <c r="S41" s="5">
+        <f t="shared" si="16"/>
+        <v>5.4780092592592597E-4</v>
+      </c>
+      <c r="T41" s="4">
+        <f t="shared" si="16"/>
+        <v>1.6953703703703702E-4</v>
+      </c>
+      <c r="U41" s="4">
+        <f t="shared" si="16"/>
+        <v>2.9918981481481479E-4</v>
+      </c>
+      <c r="V41" s="5">
+        <f t="shared" si="16"/>
+        <v>3.7121527777777777E-4</v>
+      </c>
+      <c r="W41" s="4">
+        <f t="shared" si="16"/>
+        <v>3.1687499999999999E-4</v>
+      </c>
+      <c r="X41" s="4">
+        <f t="shared" si="16"/>
+        <v>6.0594907407407407E-4</v>
+      </c>
+      <c r="Y41" s="5">
+        <f t="shared" si="16"/>
+        <v>7.4660879629629632E-4</v>
+      </c>
+      <c r="Z41" s="4">
+        <f t="shared" si="16"/>
+        <v>7.4495370370370373E-4</v>
+      </c>
+      <c r="AA41" s="4">
+        <f t="shared" si="16"/>
+        <v>1.1893287037037037E-3</v>
+      </c>
+      <c r="AB41" s="6">
+        <f t="shared" si="16"/>
+        <v>1.4789467592592593E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="42">
+        <f>(SUM(C6:E12)-SUM(Q34:S40))/SUM(C6:E12)</f>
+        <v>0.439415394744405</v>
+      </c>
+      <c r="D42" s="42"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="42">
+        <f t="shared" ref="F42" si="17">(SUM(F6:H12)-SUM(T34:V40))/SUM(F6:H12)</f>
+        <v>0.10845342080369538</v>
+      </c>
+      <c r="G42" s="42"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="42">
+        <f t="shared" ref="I42" si="18">(SUM(I6:K12)-SUM(W34:Y40))/SUM(I6:K12)</f>
+        <v>5.7027235522548084E-2</v>
+      </c>
+      <c r="J42" s="42"/>
+      <c r="K42" s="43"/>
+      <c r="L42" s="42">
+        <f t="shared" ref="L42" si="19">(SUM(L6:N12)-SUM(Z34:AB40))/SUM(L6:N12)</f>
+        <v>4.4440052103247384E-2</v>
+      </c>
+      <c r="M42" s="42"/>
+      <c r="N42" s="43"/>
+      <c r="P42" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="18">
+        <f>SUM(Q41:S41)</f>
+        <v>1.241701388888889E-3</v>
+      </c>
+      <c r="R42" s="19"/>
+      <c r="S42" s="20"/>
+      <c r="T42" s="21">
+        <f>SUM(T41:V41)</f>
+        <v>8.399421296296295E-4</v>
+      </c>
+      <c r="U42" s="19"/>
+      <c r="V42" s="20"/>
+      <c r="W42" s="21">
+        <f>SUM(W41:Y41)</f>
+        <v>1.6694328703703704E-3</v>
+      </c>
+      <c r="X42" s="19"/>
+      <c r="Y42" s="20"/>
+      <c r="Z42" s="21">
+        <f>SUM(Z41:AB41)</f>
+        <v>3.4132291666666668E-3</v>
+      </c>
+      <c r="AA42" s="19"/>
+      <c r="AB42" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="Q28:S28"/>
-    <mergeCell ref="T28:V28"/>
-    <mergeCell ref="W28:Y28"/>
-    <mergeCell ref="Z28:AB28"/>
-    <mergeCell ref="Z14:AB14"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="T4:V4"/>
-    <mergeCell ref="P16:AB16"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="T18:V18"/>
-    <mergeCell ref="W18:Y18"/>
-    <mergeCell ref="Z18:AB18"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="L18:N18"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="L28:N28"/>
+  <mergeCells count="54">
+    <mergeCell ref="Q42:S42"/>
+    <mergeCell ref="T42:V42"/>
+    <mergeCell ref="W42:Y42"/>
+    <mergeCell ref="Z42:AB42"/>
+    <mergeCell ref="B30:N30"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="L32:N32"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="I42:K42"/>
+    <mergeCell ref="L42:N42"/>
+    <mergeCell ref="P30:AB30"/>
+    <mergeCell ref="Q32:S32"/>
+    <mergeCell ref="T32:V32"/>
+    <mergeCell ref="W32:Y32"/>
+    <mergeCell ref="Z32:AB32"/>
     <mergeCell ref="B2:N2"/>
     <mergeCell ref="B16:N16"/>
     <mergeCell ref="P2:AB2"/>
@@ -2380,9 +3339,29 @@
     <mergeCell ref="Q14:S14"/>
     <mergeCell ref="T14:V14"/>
     <mergeCell ref="W14:Y14"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="L28:N28"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="T4:V4"/>
+    <mergeCell ref="P16:AB16"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="T18:V18"/>
+    <mergeCell ref="W18:Y18"/>
+    <mergeCell ref="Z18:AB18"/>
+    <mergeCell ref="Q28:S28"/>
+    <mergeCell ref="T28:V28"/>
+    <mergeCell ref="W28:Y28"/>
+    <mergeCell ref="Z28:AB28"/>
+    <mergeCell ref="Z14:AB14"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:N12">
-    <cfRule type="colorScale" priority="11">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="num" val="1000"/>
         <cfvo type="num" val="10000"/>
@@ -2394,7 +3373,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:N26">
-    <cfRule type="colorScale" priority="13">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="num" val="1000"/>
         <cfvo type="num" val="10000"/>
@@ -2406,7 +3385,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q6:AB12">
-    <cfRule type="colorScale" priority="10">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="num" val="1000"/>
         <cfvo type="num" val="10000"/>
@@ -2418,6 +3397,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q14:AB14">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="num" val="1E-3"/>
+        <cfvo type="num" val="2.5000000000000001E-3"/>
+        <cfvo type="num" val="4.0000000000000001E-3"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:N14">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="1E-3"/>
@@ -2429,8 +3420,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14:N14">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="C28:N28">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="num" val="1E-3"/>
         <cfvo type="num" val="2.5000000000000001E-3"/>
@@ -2441,7 +3432,43 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:N28">
+  <conditionalFormatting sqref="Q20:AB26">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="num" val="1000"/>
+        <cfvo type="num" val="10000"/>
+        <cfvo type="num" val="30000"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q28:AB28">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="num" val="1E-3"/>
+        <cfvo type="num" val="2.5000000000000001E-3"/>
+        <cfvo type="num" val="4.0000000000000001E-3"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q34:AB40">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="num" val="1000"/>
+        <cfvo type="num" val="10000"/>
+        <cfvo type="num" val="30000"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q42:AB42">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="1E-3"/>
@@ -2453,24 +3480,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q20:AB26">
+  <conditionalFormatting sqref="C34:N42">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="num" val="1000"/>
-        <cfvo type="num" val="10000"/>
-        <cfvo type="num" val="30000"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q28:AB28">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="num" val="1E-3"/>
-        <cfvo type="num" val="2.5000000000000001E-3"/>
-        <cfvo type="num" val="4.0000000000000001E-3"/>
+        <cfvo type="num" val="-1"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -2480,7 +3495,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C13:N13 Q27:AB27 Q13:AB13 C27:N28" formulaRange="1"/>
+    <ignoredError sqref="C13:N13 Q27:AB27 Q13:AB13 C27:N28 Q41:AB41 C41:N41" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>